<commit_message>
fix: add rights and prov statement, fix some cardinalities
</commit_message>
<xml_diff>
--- a/Formulasation(shacl)/core/Templates/SHACL-dataset-base.xlsx
+++ b/Formulasation(shacl)/core/Templates/SHACL-dataset-base.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthri-my.sharepoint.com/personal/hannah_neikes_health-ri_nl/Documents/Documenten/GDI/shacl_template_GDI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthri-my.sharepoint.com/personal/hannah_neikes_health-ri_nl/Documents/Documenten/GitHub/gdi-metadata/Formulasation(shacl)/core/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="391" documentId="13_ncr:1_{1B1DBC4C-3AF0-9940-9D98-49079FB71514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{087923DF-7325-4A43-9ED6-E4899A8EC2D7}"/>
+  <xr:revisionPtr revIDLastSave="400" documentId="13_ncr:1_{1B1DBC4C-3AF0-9940-9D98-49079FB71514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FBE97C2-787A-413D-947F-35D43CCEDB5C}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-12765" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="PropertyShapes (properties)" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'PropertyShapes (properties)'!$A$5:$X$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'PropertyShapes (properties)'!$A$5:$X$29</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="224">
   <si>
     <t>PREFIX</t>
   </si>
@@ -454,27 +454,12 @@
     <t>Properties on Dataset</t>
   </si>
   <si>
-    <t>dct:accessRights</t>
-  </si>
-  <si>
-    <t>access rights</t>
-  </si>
-  <si>
-    <t>Information that indicates whether the Dataset is publicly accessible, has access restrictions or is not public. This property must be filled with a value from a controlled vocabulary.</t>
-  </si>
-  <si>
     <t>sh:IRI</t>
   </si>
   <si>
-    <t>( eu:PUBLIC eu:RESTRICTED eu:NON_PUBLIC )</t>
-  </si>
-  <si>
     <t>dash:URIViewer</t>
   </si>
   <si>
-    <t>dash:EnumSelectEditor</t>
-  </si>
-  <si>
     <t>dash:URIEditor</t>
   </si>
   <si>
@@ -488,15 +473,6 @@
   </si>
   <si>
     <t>http://data.europa.eu/eli/reg/2025/327/oj</t>
-  </si>
-  <si>
-    <t>dcat:contactPoint</t>
-  </si>
-  <si>
-    <t>contact point</t>
-  </si>
-  <si>
-    <t>Contact information that can be used for sending comments about the Dataset.</t>
   </si>
   <si>
     <t>dash:BlankNodeEditor</t>
@@ -2362,10 +2338,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2428,7 +2404,7 @@
         <v>51</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="F1" s="3"/>
     </row>
@@ -2446,7 +2422,7 @@
         <v>54</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -2455,7 +2431,7 @@
         <v>55</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -2464,7 +2440,7 @@
         <v>56</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -2594,10 +2570,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>87</v>
@@ -2637,13 +2613,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:X36"/>
+  <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2678,7 +2654,7 @@
         <v>51</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C1" s="51"/>
       <c r="O1" s="51"/>
@@ -2877,49 +2853,51 @@
       <c r="U8" s="26"/>
       <c r="V8" s="26"/>
     </row>
-    <row r="9" spans="1:24" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="str">
-        <f t="shared" ref="A9:A31" si="0">CONCATENATE(B9,"#",SUBSTITUTE(D9," ","-"))</f>
-        <v>gdi:DatasetBaseShape#access-rights</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>230</v>
-      </c>
-      <c r="C9" s="43" t="s">
+    <row r="9" spans="1:24" s="55" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="55" t="str">
+        <f t="shared" ref="A9:A29" si="0">CONCATENATE(B9,"#",SUBSTITUTE(D9," ","-"))</f>
+        <v>gdi:DatasetBaseShape#applicable-legislation</v>
+      </c>
+      <c r="B9" s="56" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60">
+        <v>1</v>
+      </c>
+      <c r="H9" s="61"/>
+      <c r="I9" s="62" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63" t="s">
+        <v>143</v>
+      </c>
+      <c r="V9" s="63"/>
+      <c r="W9" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="X9" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="G9" s="48">
-        <v>1</v>
-      </c>
-      <c r="H9" s="49">
-        <v>1</v>
-      </c>
-      <c r="I9" s="50" t="s">
-        <v>140</v>
-      </c>
-      <c r="R9" s="51" t="s">
-        <v>141</v>
-      </c>
-      <c r="W9" s="50" t="s">
-        <v>142</v>
-      </c>
-      <c r="X9" s="50" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" s="55" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:24" s="55" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A10" s="55" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#applicable-legislation</v>
+        <v>gdi:DatasetBaseShape#creator</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C10" s="57" t="s">
         <v>145</v>
@@ -2936,28 +2914,27 @@
       </c>
       <c r="H10" s="61"/>
       <c r="I10" s="62" t="s">
-        <v>140</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="K10" s="19"/>
       <c r="S10" s="63"/>
       <c r="T10" s="63"/>
-      <c r="U10" s="63" t="s">
-        <v>148</v>
-      </c>
+      <c r="U10" s="63"/>
       <c r="V10" s="63"/>
       <c r="W10" s="62" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="X10" s="62" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#contact-point</v>
+        <v>gdi:DatasetBaseShape#description</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C11" s="43" t="s">
         <v>149</v>
@@ -2971,36 +2948,35 @@
       <c r="G11" s="48">
         <v>1</v>
       </c>
-      <c r="H11" s="49">
-        <v>1</v>
-      </c>
       <c r="I11" s="50" t="s">
-        <v>140</v>
-      </c>
-      <c r="K11" s="52"/>
+        <v>152</v>
+      </c>
+      <c r="J11" s="50" t="s">
+        <v>153</v>
+      </c>
       <c r="W11" s="50" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="X11" s="50" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:24" s="55" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A12" s="55" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#creator</v>
+        <v>gdi:DatasetBaseShape#distribution</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C12" s="57" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D12" s="57" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E12" s="58" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F12" s="59"/>
       <c r="G12" s="60">
@@ -3008,702 +2984,648 @@
       </c>
       <c r="H12" s="61"/>
       <c r="I12" s="62" t="s">
-        <v>140</v>
-      </c>
-      <c r="K12" s="19"/>
+        <v>137</v>
+      </c>
       <c r="S12" s="63"/>
       <c r="T12" s="63"/>
       <c r="U12" s="63"/>
       <c r="V12" s="63"/>
       <c r="W12" s="62" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="X12" s="62" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" ht="14.4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="72" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#description</v>
+        <v>gdi:DatasetBaseShape#health-category</v>
       </c>
       <c r="B13" s="45" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>157</v>
+        <v>205</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>158</v>
+        <v>206</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="G13" s="48">
+        <v>207</v>
+      </c>
+      <c r="G13" s="48"/>
+      <c r="I13" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="W13" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="X13" s="50" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" s="55" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="55" t="str">
+        <f>CONCATENATE(B14,"#",SUBSTITUTE(D14," ","-"))</f>
+        <v>gdi:DatasetBaseShape#health-data-access-body</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>222</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>204</v>
+      </c>
+      <c r="D14" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>209</v>
+      </c>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61">
         <v>1</v>
       </c>
-      <c r="I13" s="50" t="s">
-        <v>160</v>
-      </c>
-      <c r="J13" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="W13" s="50" t="s">
-        <v>162</v>
-      </c>
-      <c r="X13" s="50" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" s="55" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="str">
-        <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#distribution</v>
-      </c>
-      <c r="B14" s="56" t="s">
-        <v>230</v>
-      </c>
-      <c r="C14" s="57" t="s">
-        <v>164</v>
-      </c>
-      <c r="D14" s="57" t="s">
-        <v>165</v>
-      </c>
-      <c r="E14" s="58" t="s">
-        <v>166</v>
-      </c>
-      <c r="F14" s="59"/>
-      <c r="G14" s="60">
-        <v>1</v>
-      </c>
-      <c r="H14" s="61"/>
       <c r="I14" s="62" t="s">
-        <v>140</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="K14" s="19"/>
       <c r="S14" s="63"/>
       <c r="T14" s="63"/>
       <c r="U14" s="63"/>
       <c r="V14" s="63"/>
       <c r="W14" s="62" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="X14" s="62" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" ht="72" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#health-category</v>
+        <v>gdi:DatasetBaseShape#geographical-coverage</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C15" s="43" t="s">
-        <v>213</v>
+        <v>159</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>214</v>
-      </c>
-      <c r="E15" s="46" t="s">
-        <v>215</v>
-      </c>
-      <c r="G15" s="48">
-        <v>1</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>161</v>
+      </c>
+      <c r="G15" s="54"/>
       <c r="I15" s="50" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="W15" s="50" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="X15" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" s="55" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" s="55" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="55" t="str">
-        <f>CONCATENATE(B16,"#",SUBSTITUTE(D16," ","-"))</f>
-        <v>gdi:DatasetBaseShape#health-data-access-body</v>
+        <f t="shared" si="0"/>
+        <v>gdi:DatasetBaseShape#identifier</v>
       </c>
       <c r="B16" s="56" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C16" s="57" t="s">
-        <v>212</v>
+        <v>162</v>
       </c>
       <c r="D16" s="57" t="s">
-        <v>216</v>
+        <v>163</v>
       </c>
       <c r="E16" s="58" t="s">
-        <v>217</v>
+        <v>164</v>
       </c>
       <c r="F16" s="59"/>
       <c r="G16" s="60">
         <v>1</v>
       </c>
-      <c r="H16" s="61">
-        <v>1</v>
-      </c>
+      <c r="H16" s="61"/>
       <c r="I16" s="62" t="s">
-        <v>140</v>
-      </c>
-      <c r="K16" s="19"/>
+        <v>152</v>
+      </c>
+      <c r="J16" s="62"/>
       <c r="S16" s="63"/>
       <c r="T16" s="63"/>
       <c r="U16" s="63"/>
       <c r="V16" s="63"/>
       <c r="W16" s="62" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="X16" s="62" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#geographical-coverage</v>
+        <v>gdi:DatasetBaseShape#is-referenced-by</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C17" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="D17" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="E17" s="53" t="s">
-        <v>169</v>
-      </c>
-      <c r="G17" s="54">
-        <v>1</v>
-      </c>
+      <c r="G17" s="48"/>
       <c r="I17" s="50" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="W17" s="50" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="X17" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" s="55" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" s="55" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A18" s="55" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#identifier</v>
+        <v>gdi:DatasetBaseShape#keyword</v>
       </c>
       <c r="B18" s="56" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C18" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="D18" s="57" t="s">
+        <v>169</v>
+      </c>
+      <c r="E18" s="58" t="s">
         <v>170</v>
-      </c>
-      <c r="D18" s="57" t="s">
-        <v>171</v>
-      </c>
-      <c r="E18" s="58" t="s">
-        <v>172</v>
       </c>
       <c r="F18" s="59"/>
       <c r="G18" s="60">
         <v>1</v>
       </c>
-      <c r="H18" s="61">
-        <v>1</v>
-      </c>
+      <c r="H18" s="61"/>
       <c r="I18" s="62" t="s">
-        <v>160</v>
-      </c>
-      <c r="J18" s="62"/>
+        <v>152</v>
+      </c>
+      <c r="J18" s="62" t="s">
+        <v>153</v>
+      </c>
       <c r="S18" s="63"/>
       <c r="T18" s="63"/>
       <c r="U18" s="63"/>
       <c r="V18" s="63"/>
       <c r="W18" s="62" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="X18" s="62" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" ht="43.2" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#is-referenced-by</v>
+        <v>gdi:DatasetBaseShape#maximum-typical-age</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C19" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="G19" s="48"/>
+      <c r="H19" s="49">
+        <v>1</v>
+      </c>
+      <c r="I19" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="J19" s="50" t="s">
         <v>174</v>
       </c>
-      <c r="E19" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="G19" s="48"/>
-      <c r="I19" s="50" t="s">
-        <v>140</v>
-      </c>
       <c r="W19" s="50" t="s">
-        <v>142</v>
-      </c>
-      <c r="X19" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" s="55" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="X19" s="44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" s="55" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A20" s="55" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#keyword</v>
+        <v>gdi:DatasetBaseShape#minimum-typical-age</v>
       </c>
       <c r="B20" s="56" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C20" s="57" t="s">
+        <v>175</v>
+      </c>
+      <c r="D20" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="D20" s="57" t="s">
+      <c r="E20" s="58" t="s">
         <v>177</v>
       </c>
-      <c r="E20" s="58" t="s">
-        <v>178</v>
-      </c>
       <c r="F20" s="59"/>
-      <c r="G20" s="60">
+      <c r="G20" s="60"/>
+      <c r="H20" s="61">
         <v>1</v>
       </c>
-      <c r="H20" s="61"/>
       <c r="I20" s="62" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="J20" s="62" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="S20" s="63"/>
       <c r="T20" s="63"/>
       <c r="U20" s="63"/>
       <c r="V20" s="63"/>
       <c r="W20" s="62" t="s">
-        <v>162</v>
-      </c>
-      <c r="X20" s="62" t="s">
-        <v>163</v>
+        <v>154</v>
+      </c>
+      <c r="X20" s="55" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#maximum-typical-age</v>
+        <v>gdi:DatasetBaseShape#modification-date</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C21" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" s="43" t="s">
         <v>179</v>
       </c>
-      <c r="D21" s="43" t="s">
+      <c r="E21" s="46" t="s">
         <v>180</v>
-      </c>
-      <c r="E21" s="46" t="s">
-        <v>181</v>
       </c>
       <c r="G21" s="48"/>
       <c r="H21" s="49">
         <v>1</v>
       </c>
       <c r="I21" s="50" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="J21" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="V21" s="44" t="s">
         <v>182</v>
       </c>
       <c r="W21" s="50" t="s">
-        <v>162</v>
-      </c>
-      <c r="X21" s="44" t="s">
-        <v>163</v>
+        <v>154</v>
+      </c>
+      <c r="X21" s="50" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:24" s="55" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A22" s="55" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#minimum-typical-age</v>
+        <v>gdi:DatasetBaseShape#number-of-records</v>
       </c>
       <c r="B22" s="56" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C22" s="57" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D22" s="57" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E22" s="58" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F22" s="59"/>
-      <c r="G22" s="60"/>
+      <c r="G22" s="60">
+        <v>1</v>
+      </c>
       <c r="H22" s="61">
         <v>1</v>
       </c>
       <c r="I22" s="62" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="J22" s="62" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="S22" s="63"/>
       <c r="T22" s="63"/>
       <c r="U22" s="63"/>
       <c r="V22" s="63"/>
       <c r="W22" s="62" t="s">
-        <v>162</v>
-      </c>
-      <c r="X22" s="55" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="28.8" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="X22" s="62" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A23" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#modification-date</v>
+        <v>gdi:DatasetBaseShape#number-of-unique-infividuals</v>
       </c>
       <c r="B23" s="45" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C23" s="43" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D23" s="43" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G23" s="48"/>
       <c r="H23" s="49">
         <v>1</v>
       </c>
       <c r="I23" s="50" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="J23" s="50" t="s">
-        <v>189</v>
-      </c>
-      <c r="V23" s="44" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="W23" s="50" t="s">
-        <v>162</v>
-      </c>
-      <c r="X23" s="50" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" s="55" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="X23" s="44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" s="55" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A24" s="55" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#number-of-records</v>
+        <v>gdi:DatasetBaseShape#other-identifier</v>
       </c>
       <c r="B24" s="56" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C24" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="D24" s="57" t="s">
+        <v>191</v>
+      </c>
+      <c r="E24" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="D24" s="57" t="s">
-        <v>193</v>
-      </c>
-      <c r="E24" s="58" t="s">
-        <v>194</v>
-      </c>
       <c r="F24" s="59"/>
-      <c r="G24" s="60">
-        <v>1</v>
-      </c>
-      <c r="H24" s="61">
-        <v>1</v>
-      </c>
-      <c r="I24" s="62" t="s">
-        <v>160</v>
-      </c>
-      <c r="J24" s="62" t="s">
-        <v>182</v>
+      <c r="G24" s="60"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="62"/>
+      <c r="K24" s="64" t="s">
+        <v>219</v>
       </c>
       <c r="S24" s="63"/>
       <c r="T24" s="63"/>
       <c r="U24" s="63"/>
       <c r="V24" s="63"/>
-      <c r="W24" s="62" t="s">
-        <v>162</v>
-      </c>
-      <c r="X24" s="62" t="s">
-        <v>163</v>
+      <c r="W24" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="X24" s="55" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#number-of-unique-infividuals</v>
+        <v>gdi:DatasetBaseShape#HMD-submission</v>
       </c>
       <c r="B25" s="45" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C25" s="43" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="D25" s="43" t="s">
-        <v>196</v>
-      </c>
-      <c r="E25" s="46" t="s">
-        <v>197</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="E25" s="46"/>
       <c r="G25" s="48"/>
       <c r="H25" s="49">
         <v>1</v>
       </c>
       <c r="I25" s="50" t="s">
-        <v>160</v>
-      </c>
-      <c r="J25" s="50" t="s">
-        <v>182</v>
-      </c>
-      <c r="W25" s="50" t="s">
-        <v>162</v>
+        <v>137</v>
+      </c>
+      <c r="K25" s="52"/>
+      <c r="W25" s="44" t="s">
+        <v>138</v>
       </c>
       <c r="X25" s="44" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" s="55" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" s="55" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A26" s="55" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#other-identifier</v>
+        <v>gdi:DatasetBaseShape#submitter-role</v>
       </c>
       <c r="B26" s="56" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C26" s="57" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D26" s="57" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="F26" s="59"/>
       <c r="G26" s="60"/>
       <c r="H26" s="61"/>
       <c r="I26" s="62"/>
       <c r="K26" s="64" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="S26" s="63"/>
       <c r="T26" s="63"/>
       <c r="U26" s="63"/>
       <c r="V26" s="63"/>
       <c r="W26" s="55" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="X26" s="55" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" ht="14.4" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#HMD-submission</v>
+        <v>gdi:DatasetBaseShape#release-date</v>
       </c>
       <c r="B27" s="45" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C27" s="43" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="D27" s="43" t="s">
-        <v>219</v>
-      </c>
-      <c r="E27" s="46"/>
+        <v>195</v>
+      </c>
+      <c r="E27" s="46" t="s">
+        <v>196</v>
+      </c>
       <c r="G27" s="48"/>
       <c r="H27" s="49">
         <v>1</v>
       </c>
       <c r="I27" s="50" t="s">
-        <v>140</v>
-      </c>
-      <c r="K27" s="52"/>
+        <v>152</v>
+      </c>
+      <c r="J27" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="V27" s="44" t="s">
+        <v>182</v>
+      </c>
       <c r="W27" s="44" t="s">
-        <v>142</v>
-      </c>
-      <c r="X27" s="44" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" s="55" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="X27" s="50" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" s="55" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A28" s="55" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#submitter-role</v>
+        <v>gdi:DatasetBaseShape#theme</v>
       </c>
       <c r="B28" s="56" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C28" s="57" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D28" s="57" t="s">
-        <v>220</v>
+        <v>198</v>
       </c>
       <c r="E28" s="58" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
       <c r="F28" s="59"/>
-      <c r="G28" s="60"/>
+      <c r="G28" s="60">
+        <v>1</v>
+      </c>
       <c r="H28" s="61"/>
-      <c r="I28" s="62"/>
-      <c r="K28" s="64" t="s">
-        <v>228</v>
+      <c r="I28" s="62" t="s">
+        <v>137</v>
       </c>
       <c r="S28" s="63"/>
       <c r="T28" s="63"/>
-      <c r="U28" s="63"/>
+      <c r="U28" s="63" t="s">
+        <v>200</v>
+      </c>
       <c r="V28" s="63"/>
-      <c r="W28" s="55" t="s">
-        <v>156</v>
-      </c>
-      <c r="X28" s="55" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="W28" s="62" t="s">
+        <v>138</v>
+      </c>
+      <c r="X28" s="62" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#release-date</v>
+        <v>gdi:DatasetBaseShape#title</v>
       </c>
       <c r="B29" s="45" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C29" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="D29" s="43" t="s">
         <v>202</v>
       </c>
-      <c r="D29" s="43" t="s">
+      <c r="E29" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="E29" s="46" t="s">
-        <v>204</v>
-      </c>
-      <c r="G29" s="48"/>
-      <c r="H29" s="49">
+      <c r="G29" s="48">
         <v>1</v>
       </c>
       <c r="I29" s="50" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="J29" s="50" t="s">
-        <v>189</v>
-      </c>
-      <c r="V29" s="44" t="s">
-        <v>190</v>
-      </c>
-      <c r="W29" s="44" t="s">
-        <v>162</v>
+        <v>153</v>
+      </c>
+      <c r="W29" s="50" t="s">
+        <v>154</v>
       </c>
       <c r="X29" s="50" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" s="55" customFormat="1" ht="72" x14ac:dyDescent="0.25">
-      <c r="A30" s="55" t="str">
-        <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#theme</v>
-      </c>
-      <c r="B30" s="56" t="s">
-        <v>230</v>
-      </c>
-      <c r="C30" s="57" t="s">
-        <v>205</v>
-      </c>
-      <c r="D30" s="57" t="s">
-        <v>206</v>
-      </c>
-      <c r="E30" s="58" t="s">
-        <v>207</v>
-      </c>
-      <c r="F30" s="59"/>
-      <c r="G30" s="60">
-        <v>1</v>
-      </c>
-      <c r="H30" s="61"/>
-      <c r="I30" s="62" t="s">
-        <v>140</v>
-      </c>
-      <c r="S30" s="63"/>
-      <c r="T30" s="63"/>
-      <c r="U30" s="63" t="s">
-        <v>208</v>
-      </c>
-      <c r="V30" s="63"/>
-      <c r="W30" s="62" t="s">
-        <v>142</v>
-      </c>
-      <c r="X30" s="62" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A31" s="44" t="str">
-        <f t="shared" si="0"/>
-        <v>gdi:DatasetBaseShape#title</v>
-      </c>
-      <c r="B31" s="45" t="s">
-        <v>230</v>
-      </c>
-      <c r="C31" s="43" t="s">
-        <v>209</v>
-      </c>
-      <c r="D31" s="43" t="s">
-        <v>210</v>
-      </c>
-      <c r="E31" s="46" t="s">
-        <v>211</v>
-      </c>
-      <c r="G31" s="48">
-        <v>1</v>
-      </c>
-      <c r="I31" s="50" t="s">
-        <v>160</v>
-      </c>
-      <c r="J31" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="W31" s="50" t="s">
-        <v>162</v>
-      </c>
-      <c r="X31" s="50" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" s="80" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" s="80" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B30" s="81"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="84"/>
+      <c r="I30" s="85"/>
+      <c r="S30" s="82"/>
+      <c r="T30" s="82"/>
+      <c r="U30" s="82"/>
+      <c r="V30" s="82"/>
+      <c r="W30" s="85"/>
+      <c r="X30" s="85"/>
+    </row>
+    <row r="31" spans="1:24" s="80" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B31" s="81"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="83"/>
+      <c r="G31" s="87"/>
+      <c r="H31" s="84"/>
+      <c r="S31" s="82"/>
+      <c r="T31" s="82"/>
+      <c r="U31" s="82"/>
+      <c r="V31" s="82"/>
+    </row>
+    <row r="32" spans="1:24" s="80" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="81"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
+      <c r="D32" s="86"/>
       <c r="E32" s="82"/>
       <c r="F32" s="83"/>
-      <c r="G32" s="30"/>
+      <c r="G32" s="87"/>
       <c r="H32" s="84"/>
-      <c r="I32" s="85"/>
       <c r="S32" s="82"/>
       <c r="T32" s="82"/>
       <c r="U32" s="82"/>
       <c r="V32" s="82"/>
-      <c r="W32" s="85"/>
-      <c r="X32" s="85"/>
     </row>
     <row r="33" spans="2:22" s="80" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="81"/>
@@ -3729,42 +3651,17 @@
       <c r="U34" s="82"/>
       <c r="V34" s="82"/>
     </row>
-    <row r="35" spans="2:22" s="80" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B35" s="81"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="82"/>
-      <c r="F35" s="83"/>
-      <c r="G35" s="87"/>
-      <c r="H35" s="84"/>
-      <c r="S35" s="82"/>
-      <c r="T35" s="82"/>
-      <c r="U35" s="82"/>
-      <c r="V35" s="82"/>
-    </row>
-    <row r="36" spans="2:22" s="80" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B36" s="81"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="82"/>
-      <c r="F36" s="83"/>
-      <c r="G36" s="87"/>
-      <c r="H36" s="84"/>
-      <c r="S36" s="82"/>
-      <c r="T36" s="82"/>
-      <c r="U36" s="82"/>
-      <c r="V36" s="82"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A5:X31" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A5:X29" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="K12" r:id="rId2" display="http://data.health-ri.nl/GDI/AgentBaseShape" xr:uid="{759F7A40-6F19-4F37-AAD0-6519B1218587}"/>
-    <hyperlink ref="K28" r:id="rId3" xr:uid="{AC22EB73-D311-4396-AA13-488A77DB9AB8}"/>
-    <hyperlink ref="K26" r:id="rId4" xr:uid="{FEF62B8F-6A55-4FEC-9D65-E134068B0AAC}"/>
-    <hyperlink ref="K11" r:id="rId5" display="http://data.health-ri.nl/GDI/KindShape" xr:uid="{CD3BDA36-060A-4F93-B408-F72345F4BFB4}"/>
-    <hyperlink ref="K16" r:id="rId6" display="http://data.health-ri.nl/GDI/AgentBaseShape" xr:uid="{A89BF0E9-8340-4ADD-A5C5-3AA2FFAE98A5}"/>
+    <hyperlink ref="K10" r:id="rId2" display="http://data.health-ri.nl/GDI/AgentBaseShape" xr:uid="{759F7A40-6F19-4F37-AAD0-6519B1218587}"/>
+    <hyperlink ref="K26" r:id="rId3" xr:uid="{AC22EB73-D311-4396-AA13-488A77DB9AB8}"/>
+    <hyperlink ref="K24" r:id="rId4" xr:uid="{FEF62B8F-6A55-4FEC-9D65-E134068B0AAC}"/>
+    <hyperlink ref="K14" r:id="rId5" display="http://data.health-ri.nl/GDI/AgentBaseShape" xr:uid="{A89BF0E9-8340-4ADD-A5C5-3AA2FFAE98A5}"/>
   </hyperlinks>
   <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="1.05277777777778" bottom="1.05277777777778" header="0.78750000000000009" footer="0.78750000000000009"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -3773,24 +3670,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
-    <Categorie xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
-    <Persoon xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Persoon>
-    <Opmerkingen xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4082,21 +3967,30 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
+    <Categorie xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
+    <Persoon xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Persoon>
+    <Opmerkingen xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D188C3D5-44E3-4A45-B4C8-A1EF171C14AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{714965F3-B175-40D4-A6BA-6E5740C5D9B2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
-    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4121,9 +4015,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{714965F3-B175-40D4-A6BA-6E5740C5D9B2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D188C3D5-44E3-4A45-B4C8-A1EF171C14AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
+    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>